<commit_message>
Working on refactoring group counts
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>NZ7l</x:t>
+    <x:t>zoSB</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -91,7 +91,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>qk64</x:t>
+    <x:t>MrYf</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -109,7 +109,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>t0xs</x:t>
+    <x:t>h7gL</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -122,7 +122,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>zt1S</x:t>
+    <x:t>jow9</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -135,7 +135,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>EXOZ</x:t>
+    <x:t>PUQh</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -148,7 +148,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>r7Bg</x:t>
+    <x:t>LUYG</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -161,7 +161,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>qQNc</x:t>
+    <x:t>Gf0M</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -176,7 +176,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>Nccr</x:t>
+    <x:t>NiRn</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -188,7 +188,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>q10f</x:t>
+    <x:t>LeCq</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_CO2Z</x:t>
@@ -203,7 +203,7 @@
     <x:t>Hi, Laura here. What's up?</x:t>
   </x:si>
   <x:si>
-    <x:t>aWxE</x:t>
+    <x:t>QMwJ</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_5T8A</x:t>
@@ -219,7 +219,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>b5Ik</x:t>
+    <x:t>sHOs</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -231,7 +231,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>Xsmw</x:t>
+    <x:t>lGAB</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -243,7 +243,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>3yqd</x:t>
+    <x:t>kO4u</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -255,7 +255,7 @@
     <x:t>(3/3) Really mean it!</x:t>
   </x:si>
   <x:si>
-    <x:t>DYZQ</x:t>
+    <x:t>gZxI</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -271,7 +271,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>y7w1</x:t>
+    <x:t>utPz</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -321,7 +321,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>sra9</x:t>
+    <x:t>XrkT</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -333,7 +333,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>mExv</x:t>
+    <x:t>4L9m</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -345,7 +345,7 @@
     <x:t>(3/7) How about this?</x:t>
   </x:si>
   <x:si>
-    <x:t>LoFV</x:t>
+    <x:t>vdSU</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -357,7 +357,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>zTwT</x:t>
+    <x:t>l5L4</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -369,7 +369,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>t343</x:t>
+    <x:t>iNj4</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -396,7 +396,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>UbQH</x:t>
+    <x:t>bDdo</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -408,7 +408,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>olFJ</x:t>
+    <x:t>0r0f</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Finish refactor of snippet grouping.
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>IWdy</x:t>
+    <x:t>uXOa</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -91,7 +91,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>zZ8o</x:t>
+    <x:t>N3Ke</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -109,7 +109,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>ZIf7</x:t>
+    <x:t>9Xte</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -122,7 +122,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>O39G</x:t>
+    <x:t>Bpuz</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -135,7 +135,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>wIjn</x:t>
+    <x:t>8KkF</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -148,7 +148,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>l70x</x:t>
+    <x:t>igag</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -161,7 +161,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>2uOq</x:t>
+    <x:t>uQLC</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -176,7 +176,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>bENa</x:t>
+    <x:t>5N0e</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -188,7 +188,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>g7QL</x:t>
+    <x:t>I2Ri</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_CO2Z</x:t>
@@ -207,7 +207,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Y94A</x:t>
+    <x:t>7cC0</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_5T8A</x:t>
@@ -223,7 +223,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>H8CC</x:t>
+    <x:t>d5aj</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -235,7 +235,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>1ZnP</x:t>
+    <x:t>AJbt</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -247,7 +247,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>wbeV</x:t>
+    <x:t>QxNF</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -259,7 +259,7 @@
     <x:t>(3/3) Really mean it!</x:t>
   </x:si>
   <x:si>
-    <x:t>MBNA</x:t>
+    <x:t>uR5r</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -277,7 +277,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>X2VI</x:t>
+    <x:t>zyiY</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -327,7 +327,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>pOMH</x:t>
+    <x:t>1gvn</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -339,7 +339,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>OWPJ</x:t>
+    <x:t>pnRQ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -351,7 +351,7 @@
     <x:t>(3/7) How about this?</x:t>
   </x:si>
   <x:si>
-    <x:t>nQK7</x:t>
+    <x:t>arGM</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -363,7 +363,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>XwRg</x:t>
+    <x:t>m7xl</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -375,7 +375,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>x0s5</x:t>
+    <x:t>ky8X</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -402,7 +402,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>zKgw</x:t>
+    <x:t>roOK</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -414,7 +414,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>rXaB</x:t>
+    <x:t>oUh7</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Get origins from Localiser.
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>YuH1</x:t>
+    <x:t>B7t5</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -91,7 +91,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>iX2Q</x:t>
+    <x:t>jd0f</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -109,7 +109,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>b1mO</x:t>
+    <x:t>1G55</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -122,7 +122,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Iafa</x:t>
+    <x:t>386V</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -135,7 +135,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>iGoy</x:t>
+    <x:t>Rfvk</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -148,7 +148,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>dfLd</x:t>
+    <x:t>rVib</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -161,7 +161,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>uJUA</x:t>
+    <x:t>xgUi</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -176,7 +176,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>EXMY</x:t>
+    <x:t>11u1</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -188,7 +188,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>FZE6</x:t>
+    <x:t>G6G4</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_CO2Z</x:t>
@@ -203,7 +203,7 @@
     <x:t>Hi, Laura here. What's up?</x:t>
   </x:si>
   <x:si>
-    <x:t>Ndgo</x:t>
+    <x:t>18Wn</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_5T8A</x:t>
@@ -219,7 +219,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>3qmz</x:t>
+    <x:t>6IAN</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -232,7 +232,7 @@
 (1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>SlY1</x:t>
+    <x:t>ejHV</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -244,7 +244,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>sPmp</x:t>
+    <x:t>8qLB</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -256,7 +256,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>Iep7</x:t>
+    <x:t>twHV</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -272,7 +272,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>RwSy</x:t>
+    <x:t>Sl7I</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -322,7 +322,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>VPdF</x:t>
+    <x:t>VnUX</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -334,7 +334,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>YKom</x:t>
+    <x:t>BUhZ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -346,7 +346,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>xUFU</x:t>
+    <x:t>BuRx</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -358,7 +358,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>v685</x:t>
+    <x:t>u7lc</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -370,7 +370,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>wFYQ</x:t>
+    <x:t>k9fF</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -397,7 +397,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>gomc</x:t>
+    <x:t>0twZ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -409,7 +409,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>a5CI</x:t>
+    <x:t>ONXm</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Add text content stripping.
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>B7t5</x:t>
+    <x:t>w7zp</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -91,7 +91,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>jd0f</x:t>
+    <x:t>D5hS</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -109,7 +109,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>1G55</x:t>
+    <x:t>WSyU</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -122,7 +122,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>386V</x:t>
+    <x:t>aaR0</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -135,7 +135,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Rfvk</x:t>
+    <x:t>YDaQ</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -148,7 +148,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>rVib</x:t>
+    <x:t>blNR</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -161,7 +161,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>xgUi</x:t>
+    <x:t>GX53</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -176,7 +176,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>11u1</x:t>
+    <x:t>nvdw</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -188,7 +188,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>G6G4</x:t>
+    <x:t>SlpG</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_CO2Z</x:t>
@@ -203,7 +203,7 @@
     <x:t>Hi, Laura here. What's up?</x:t>
   </x:si>
   <x:si>
-    <x:t>18Wn</x:t>
+    <x:t>sd2u</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_5T8A</x:t>
@@ -219,7 +219,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>6IAN</x:t>
+    <x:t>LTD9</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -232,7 +232,7 @@
 (1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>ejHV</x:t>
+    <x:t>wEui</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -244,7 +244,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>8qLB</x:t>
+    <x:t>GVje</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -256,7 +256,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>twHV</x:t>
+    <x:t>7inI</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -272,7 +272,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>Sl7I</x:t>
+    <x:t>y2Bv</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -322,7 +322,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>VnUX</x:t>
+    <x:t>hUaM</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -334,7 +334,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>BUhZ</x:t>
+    <x:t>lAkH</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -346,7 +346,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>BuRx</x:t>
+    <x:t>PSMq</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -358,7 +358,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>u7lc</x:t>
+    <x:t>xSfR</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -370,7 +370,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>k9fF</x:t>
+    <x:t>U06q</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -397,7 +397,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>0twZ</x:t>
+    <x:t>EhGW</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -409,7 +409,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>ONXm</x:t>
+    <x:t>ylr1</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Fix issues with LocaliserTool
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>YM10</x:t>
+    <x:t>w7zp</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -91,7 +91,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>DD4S</x:t>
+    <x:t>D5hS</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -109,7 +109,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>o0OZ</x:t>
+    <x:t>WSyU</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -122,7 +122,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>oAg3</x:t>
+    <x:t>aaR0</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -135,7 +135,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>BrfI</x:t>
+    <x:t>YDaQ</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -148,7 +148,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>kjLg</x:t>
+    <x:t>blNR</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -161,7 +161,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>7v2L</x:t>
+    <x:t>GX53</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -176,7 +176,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>7gTH</x:t>
+    <x:t>nvdw</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -188,7 +188,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>oJ5H</x:t>
+    <x:t>SlpG</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_CO2Z</x:t>
@@ -203,7 +203,7 @@
     <x:t>Hi, Laura here. What's up?</x:t>
   </x:si>
   <x:si>
-    <x:t>ffgc</x:t>
+    <x:t>sd2u</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_5T8A</x:t>
@@ -219,7 +219,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>7qbK</x:t>
+    <x:t>LTD9</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -232,7 +232,7 @@
 (1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>fpQw</x:t>
+    <x:t>wEui</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -244,7 +244,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>i7O0</x:t>
+    <x:t>GVje</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -256,7 +256,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>I7HR</x:t>
+    <x:t>7inI</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -272,7 +272,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>XFJg</x:t>
+    <x:t>y2Bv</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -322,7 +322,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>4W2d</x:t>
+    <x:t>hUaM</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -334,7 +334,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>bCvh</x:t>
+    <x:t>lAkH</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -346,7 +346,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Ji0g</x:t>
+    <x:t>PSMq</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -358,7 +358,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>RT21</x:t>
+    <x:t>xSfR</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -370,7 +370,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>75XB</x:t>
+    <x:t>U06q</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -397,7 +397,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>FZVZ</x:t>
+    <x:t>EhGW</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -409,7 +409,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Zl0I</x:t>
+    <x:t>ylr1</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Add some parser testing.
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -61,7 +61,7 @@
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>xrCj</x:t>
+    <x:t>pRc8</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -80,7 +80,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Ng99</x:t>
+    <x:t>jYRk</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -93,7 +93,7 @@
 (1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>dYqx</x:t>
+    <x:t>44Bu</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -105,7 +105,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>7jHP</x:t>
+    <x:t>fS1D</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -117,7 +117,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>rju7</x:t>
+    <x:t>2qVk</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -133,7 +133,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>ltTb</x:t>
+    <x:t>Mt0v</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -189,7 +189,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>AhmM</x:t>
+    <x:t>9jkf</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -201,7 +201,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>sv3X</x:t>
+    <x:t>7ugC</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -213,7 +213,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>3eFd</x:t>
+    <x:t>TDsX</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -225,7 +225,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>6PPO</x:t>
+    <x:t>qcyb</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -237,7 +237,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>8qfr</x:t>
+    <x:t>c8Ox</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -264,7 +264,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>IsSk</x:t>
+    <x:t>J12J</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -276,7 +276,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>NA0w</x:t>
+    <x:t>Tt3X</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part1_S494</x:t>
@@ -288,7 +288,7 @@
     <x:t>This is a block called Part1 in a scene.</x:t>
   </x:si>
   <x:si>
-    <x:t>hnEq</x:t>
+    <x:t>VWFS</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part1_ICIG</x:t>
@@ -312,7 +312,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>c8Dr</x:t>
+    <x:t>lAhm</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -330,7 +330,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>05Th</x:t>
+    <x:t>bE3k</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -343,7 +343,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>dPGP</x:t>
+    <x:t>sU8t</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -356,7 +356,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>efn4</x:t>
+    <x:t>QCZl</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -369,7 +369,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>hKWW</x:t>
+    <x:t>NB3S</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -382,7 +382,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>MBZQ</x:t>
+    <x:t>v3O6</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -397,7 +397,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>mdoK</x:t>
+    <x:t>THo6</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -409,7 +409,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>rH1O</x:t>
+    <x:t>4q8u</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Finding a more stable SnippetID
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-recording.xlsx
+++ b/examples/test-js/dink-content/main-recording.xlsx
@@ -61,7 +61,7 @@
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>LI2i</x:t>
+    <x:t>YkTdef</x:t>
   </x:si>
   <x:si>
     <x:t>Unknown</x:t>
@@ -80,7 +80,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>14hw</x:t>
+    <x:t>chW8xg</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_J0MK</x:t>
@@ -93,7 +93,7 @@
 (1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>Iu7g</x:t>
+    <x:t>jZ2lVG</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_CIMX</x:t>
@@ -105,7 +105,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>MdR8</x:t>
+    <x:t>PXBE7j</x:t>
   </x:si>
   <x:si>
     <x:t>main_LauraChat_Hub_L3K7</x:t>
@@ -117,7 +117,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>QeZy</x:t>
+    <x:t>DvVSQ6</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -133,7 +133,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>bsX4</x:t>
+    <x:t>qQOReF</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_G33S</x:t>
@@ -189,7 +189,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>vuhJ</x:t>
+    <x:t>iZ38Lw</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -201,7 +201,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>DslZ</x:t>
+    <x:t>32hKE1</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -213,7 +213,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>cqPF</x:t>
+    <x:t>U30VuF</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -225,7 +225,7 @@
     <x:t xml:space="preserve">(4/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>inIQ</x:t>
+    <x:t>i1GMUb</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_4444</x:t>
@@ -237,7 +237,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>3TbQ</x:t>
+    <x:t>MdGHyj</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -264,7 +264,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Fdsi</x:t>
+    <x:t>15ftGt</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -276,7 +276,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>JF87</x:t>
+    <x:t>bbXZ4o</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part1_S494</x:t>
@@ -288,7 +288,7 @@
     <x:t>This is a block called Part1 in a scene.</x:t>
   </x:si>
   <x:si>
-    <x:t>bXzO</x:t>
+    <x:t>9YpLlu</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part1_ICIG</x:t>
@@ -312,7 +312,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>EYip</x:t>
+    <x:t>kRZMEF</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_NY6V</x:t>
@@ -330,7 +330,7 @@
     <x:t>There is a choice here.</x:t>
   </x:si>
   <x:si>
-    <x:t>77CJ</x:t>
+    <x:t>AQWHIa</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -343,7 +343,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>0olR</x:t>
+    <x:t>xo4coL</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -356,7 +356,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>yydv</x:t>
+    <x:t>BZAGzy</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -369,7 +369,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>YQvi</x:t>
+    <x:t>IkrPq2</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -382,7 +382,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>veTB</x:t>
+    <x:t>lTztHz</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -397,7 +397,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>X6va</x:t>
+    <x:t>0pCnXe</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -409,7 +409,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>hUNn</x:t>
+    <x:t>GBmTaQ</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>